<commit_message>
poisson_naive pronta para a rodada 27
</commit_message>
<xml_diff>
--- a/dados/historico/times/rodada_26/America (MG).xlsx
+++ b/dados/historico/times/rodada_26/America (MG).xlsx
@@ -712,7 +712,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>246</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -729,10 +729,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Matchweek 1</t>
-        </is>
+      <c r="E2" t="n">
+        <v>1</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -900,7 +898,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>247</v>
+        <v>6</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -917,10 +915,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Matchweek 4</t>
-        </is>
+      <c r="E3" t="n">
+        <v>4</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -1088,7 +1084,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>248</v>
+        <v>8</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1105,10 +1101,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Matchweek 6</t>
-        </is>
+      <c r="E4" t="n">
+        <v>6</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -1276,7 +1270,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>249</v>
+        <v>9</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1293,10 +1287,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Matchweek 7</t>
-        </is>
+      <c r="E5" t="n">
+        <v>7</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -1464,7 +1456,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>250</v>
+        <v>12</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -1481,10 +1473,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Matchweek 9</t>
-        </is>
+      <c r="E6" t="n">
+        <v>9</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -1652,7 +1642,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>251</v>
+        <v>14</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -1669,10 +1659,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Matchweek 10</t>
-        </is>
+      <c r="E7" t="n">
+        <v>10</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -1840,7 +1828,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>252</v>
+        <v>16</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1857,10 +1845,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Matchweek 12</t>
-        </is>
+      <c r="E8" t="n">
+        <v>12</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -2028,7 +2014,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>253</v>
+        <v>23</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -2045,10 +2031,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Matchweek 17</t>
-        </is>
+      <c r="E9" t="n">
+        <v>17</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -2214,7 +2198,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>254</v>
+        <v>27</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -2231,10 +2215,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Matchweek 19</t>
-        </is>
+      <c r="E10" t="n">
+        <v>19</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -2400,7 +2382,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>255</v>
+        <v>30</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -2417,10 +2399,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Matchweek 21</t>
-        </is>
+      <c r="E11" t="n">
+        <v>21</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -2586,7 +2566,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>256</v>
+        <v>32</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -2603,10 +2583,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Matchweek 22</t>
-        </is>
+      <c r="E12" t="n">
+        <v>22</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -2772,7 +2750,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>257</v>
+        <v>34</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -2789,10 +2767,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Matchweek 24</t>
-        </is>
+      <c r="E13" t="n">
+        <v>24</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -2958,7 +2934,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>258</v>
+        <v>35</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -2975,10 +2951,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Matchweek 15</t>
-        </is>
+      <c r="E14" t="n">
+        <v>15</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -3144,7 +3118,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -3161,10 +3135,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Matchweek 8</t>
-        </is>
+      <c r="E15" t="n">
+        <v>8</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -3332,7 +3304,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -3349,10 +3321,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Matchweek 5</t>
-        </is>
+      <c r="E16" t="n">
+        <v>5</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -3520,7 +3490,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -3537,10 +3507,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Matchweek 11</t>
-        </is>
+      <c r="E17" t="n">
+        <v>11</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -3708,7 +3676,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -3725,10 +3693,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Matchweek 16</t>
-        </is>
+      <c r="E18" t="n">
+        <v>16</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -3894,7 +3860,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -3911,10 +3877,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Matchweek 26</t>
-        </is>
+      <c r="E19" t="n">
+        <v>26</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -4080,7 +4044,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -4097,10 +4061,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Matchweek 20</t>
-        </is>
+      <c r="E20" t="n">
+        <v>20</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -4266,7 +4228,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -4283,10 +4245,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Matchweek 13</t>
-        </is>
+      <c r="E21" t="n">
+        <v>13</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -4454,7 +4414,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>118</v>
+        <v>3</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -4471,10 +4431,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Matchweek 2</t>
-        </is>
+      <c r="E22" t="n">
+        <v>2</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -4642,7 +4600,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>142</v>
+        <v>22</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -4659,10 +4617,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Matchweek 23</t>
-        </is>
+      <c r="E23" t="n">
+        <v>23</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -4828,16 +4784,16 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>171</v>
+        <v>24</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2023-04-29</t>
+          <t>2023-10-01</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>18:30</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -4845,14 +4801,12 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Matchweek 3</t>
-        </is>
+      <c r="E24" t="n">
+        <v>25</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Sat</t>
+          <t>Sun</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -4862,14 +4816,14 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>D</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
@@ -4877,155 +4831,153 @@
         </is>
       </c>
       <c r="L24" t="n">
-        <v>1.8</v>
+        <v>0.6</v>
       </c>
       <c r="M24" t="n">
-        <v>1.8</v>
+        <v>1</v>
       </c>
       <c r="N24" t="n">
-        <v>44</v>
-      </c>
-      <c r="O24" t="n">
-        <v>11844</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="O24" t="inlineStr"/>
       <c r="P24" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="Q24" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="R24" t="n">
-        <v>45.5</v>
+        <v>11.8</v>
       </c>
       <c r="S24" t="n">
-        <v>0.18</v>
+        <v>0.06</v>
       </c>
       <c r="T24" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="U24" t="n">
+        <v>0</v>
+      </c>
+      <c r="V24" t="n">
+        <v>0</v>
+      </c>
+      <c r="W24" t="n">
+        <v>0</v>
+      </c>
+      <c r="X24" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="Z24" t="n">
         <v>0.4</v>
       </c>
-      <c r="U24" t="n">
-        <v>1</v>
-      </c>
-      <c r="V24" t="n">
-        <v>1</v>
-      </c>
-      <c r="W24" t="n">
-        <v>1</v>
-      </c>
-      <c r="X24" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y24" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="Z24" t="n">
-        <v>1.2</v>
-      </c>
       <c r="AA24" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="AB24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AC24" t="n">
         <v>6</v>
       </c>
       <c r="AD24" t="n">
-        <v>75</v>
+        <v>85.7</v>
       </c>
       <c r="AE24" t="n">
         <v>0</v>
       </c>
       <c r="AF24" t="n">
-        <v>2.9</v>
+        <v>1.3</v>
       </c>
       <c r="AG24" t="n">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="AH24" t="n">
-        <v>4196</v>
+        <v>8317</v>
       </c>
       <c r="AI24" t="n">
-        <v>1827</v>
+        <v>2814</v>
       </c>
       <c r="AJ24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK24" t="n">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="AL24" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="AM24" t="n">
+        <v>15</v>
+      </c>
+      <c r="AN24" t="n">
+        <v>39</v>
+      </c>
+      <c r="AO24" t="n">
+        <v>10</v>
+      </c>
+      <c r="AP24" t="n">
+        <v>4</v>
+      </c>
+      <c r="AQ24" t="n">
+        <v>51</v>
+      </c>
+      <c r="AR24" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT24" t="n">
+        <v>27</v>
+      </c>
+      <c r="AU24" t="n">
+        <v>10</v>
+      </c>
+      <c r="AV24" t="n">
+        <v>33</v>
+      </c>
+      <c r="AW24" t="n">
+        <v>2</v>
+      </c>
+      <c r="AX24" t="n">
         <v>9</v>
       </c>
-      <c r="AN24" t="n">
-        <v>24</v>
-      </c>
-      <c r="AO24" t="n">
-        <v>5</v>
-      </c>
-      <c r="AP24" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ24" t="n">
-        <v>25</v>
-      </c>
-      <c r="AR24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS24" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT24" t="n">
-        <v>17</v>
-      </c>
-      <c r="AU24" t="n">
-        <v>8</v>
-      </c>
-      <c r="AV24" t="n">
-        <v>22</v>
-      </c>
-      <c r="AW24" t="n">
-        <v>5</v>
-      </c>
-      <c r="AX24" t="n">
-        <v>7</v>
-      </c>
       <c r="AY24" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AZ24" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="BA24" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BB24" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="BC24" t="n">
         <v>0</v>
       </c>
       <c r="BD24" t="inlineStr">
         <is>
-          <t>Santos</t>
+          <t>Cruzeiro</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>195</v>
+        <v>4</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2023-10-01</t>
+          <t>2023-04-29</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>18:30</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -5033,14 +4985,12 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Matchweek 25</t>
-        </is>
+      <c r="E25" t="n">
+        <v>3</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Sun</t>
+          <t>Sat</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -5050,14 +5000,14 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>W</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
@@ -5065,144 +5015,146 @@
         </is>
       </c>
       <c r="L25" t="n">
-        <v>0.6</v>
+        <v>1.8</v>
       </c>
       <c r="M25" t="n">
-        <v>1</v>
+        <v>1.8</v>
       </c>
       <c r="N25" t="n">
-        <v>59</v>
-      </c>
-      <c r="O25" t="inlineStr"/>
+        <v>44</v>
+      </c>
+      <c r="O25" t="n">
+        <v>11844</v>
+      </c>
       <c r="P25" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="Q25" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R25" t="n">
-        <v>11.8</v>
+        <v>45.5</v>
       </c>
       <c r="S25" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
       <c r="T25" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X25" t="n">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="Y25" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="Z25" t="n">
-        <v>0.4</v>
+        <v>1.2</v>
       </c>
       <c r="AA25" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AB25" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC25" t="n">
         <v>6</v>
       </c>
       <c r="AD25" t="n">
-        <v>85.7</v>
+        <v>75</v>
       </c>
       <c r="AE25" t="n">
         <v>0</v>
       </c>
       <c r="AF25" t="n">
-        <v>1.3</v>
+        <v>2.9</v>
       </c>
       <c r="AG25" t="n">
-        <v>0.3</v>
+        <v>0.9</v>
       </c>
       <c r="AH25" t="n">
-        <v>8317</v>
+        <v>4196</v>
       </c>
       <c r="AI25" t="n">
-        <v>2814</v>
+        <v>1827</v>
       </c>
       <c r="AJ25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK25" t="n">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="AL25" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="AM25" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="AN25" t="n">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="AO25" t="n">
+        <v>5</v>
+      </c>
+      <c r="AP25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ25" t="n">
+        <v>25</v>
+      </c>
+      <c r="AR25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT25" t="n">
+        <v>17</v>
+      </c>
+      <c r="AU25" t="n">
+        <v>8</v>
+      </c>
+      <c r="AV25" t="n">
+        <v>22</v>
+      </c>
+      <c r="AW25" t="n">
+        <v>5</v>
+      </c>
+      <c r="AX25" t="n">
+        <v>7</v>
+      </c>
+      <c r="AY25" t="n">
+        <v>3</v>
+      </c>
+      <c r="AZ25" t="n">
+        <v>11</v>
+      </c>
+      <c r="BA25" t="n">
+        <v>3</v>
+      </c>
+      <c r="BB25" t="n">
         <v>10</v>
       </c>
-      <c r="AP25" t="n">
-        <v>4</v>
-      </c>
-      <c r="AQ25" t="n">
-        <v>51</v>
-      </c>
-      <c r="AR25" t="n">
-        <v>2</v>
-      </c>
-      <c r="AS25" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT25" t="n">
-        <v>27</v>
-      </c>
-      <c r="AU25" t="n">
-        <v>10</v>
-      </c>
-      <c r="AV25" t="n">
-        <v>33</v>
-      </c>
-      <c r="AW25" t="n">
-        <v>2</v>
-      </c>
-      <c r="AX25" t="n">
-        <v>9</v>
-      </c>
-      <c r="AY25" t="n">
-        <v>4</v>
-      </c>
-      <c r="AZ25" t="n">
-        <v>10</v>
-      </c>
-      <c r="BA25" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB25" t="n">
-        <v>12</v>
-      </c>
       <c r="BC25" t="n">
         <v>0</v>
       </c>
       <c r="BD25" t="inlineStr">
         <is>
-          <t>Cruzeiro</t>
+          <t>Santos</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>204</v>
+        <v>17</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -5219,10 +5171,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Matchweek 18</t>
-        </is>
+      <c r="E26" t="n">
+        <v>18</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -5390,7 +5340,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>240</v>
+        <v>13</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -5407,10 +5357,8 @@
           <t>Série A</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Matchweek 14</t>
-        </is>
+      <c r="E27" t="n">
+        <v>14</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
poisson_naive versao media ponderada
</commit_message>
<xml_diff>
--- a/dados/historico/times/rodada_26/America (MG).xlsx
+++ b/dados/historico/times/rodada_26/America (MG).xlsx
@@ -712,7 +712,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>494</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -898,7 +898,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>6</v>
+        <v>497</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>8</v>
+        <v>499</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1270,7 +1270,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>9</v>
+        <v>500</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1456,7 +1456,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>12</v>
+        <v>502</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -1642,7 +1642,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>14</v>
+        <v>503</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -1828,7 +1828,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>16</v>
+        <v>505</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -2014,7 +2014,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>23</v>
+        <v>509</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -2198,7 +2198,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>27</v>
+        <v>511</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -2382,7 +2382,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>30</v>
+        <v>513</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -2566,7 +2566,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>32</v>
+        <v>514</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -2750,7 +2750,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>34</v>
+        <v>516</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -2934,7 +2934,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>35</v>
+        <v>517</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -3118,7 +3118,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -3304,7 +3304,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -3490,7 +3490,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -3676,7 +3676,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>21</v>
+        <v>119</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -3860,7 +3860,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>41</v>
+        <v>155</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -4044,7 +4044,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>27</v>
+        <v>175</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -4228,7 +4228,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>22</v>
+        <v>220</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -4414,7 +4414,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>3</v>
+        <v>235</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -4600,7 +4600,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>22</v>
+        <v>282</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -4784,7 +4784,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>24</v>
+        <v>336</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -4968,7 +4968,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>4</v>
+        <v>366</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -5154,7 +5154,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>17</v>
+        <v>407</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -5340,7 +5340,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>13</v>
+        <v>481</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>

</xml_diff>